<commit_message>
feat(IntensitasFilter): add conditional formatting based on persil data
Implement dynamic data grouping and formatting in IntensitasFilter component to handle both persil (location-specific) and non-persil data cases. The component now checks for persil data and adjusts the output format accordingly for building height and setback line values.
</commit_message>
<xml_diff>
--- a/app/data/kepsus/kepsus.xlsx
+++ b/app/data/kepsus/kepsus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\le\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\le\Downloads\RDTR BUILDER TRIKORA\rdtr-filter-app\app\data\kepsus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E51F1D-F0ED-45FF-A0C0-F2B78132C8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2E6141-E49A-4951-9EEE-6EFE3853EC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{638C47D1-A81B-4105-B767-5B7061BB285E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{638C47D1-A81B-4105-B767-5B7061BB285E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3439" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3439" uniqueCount="459">
   <si>
     <t>TABEL KETENTUAN KHUSUS KAWASAN KESELAMATAN OPERASI PENERBANGAN</t>
   </si>
@@ -1466,6 +1466,9 @@
   </si>
   <si>
     <t>Tabel</t>
+  </si>
+  <si>
+    <t>Rawan Bencana Cuaca Ekstrem Tingkat Tinggi</t>
   </si>
 </sst>
 </file>
@@ -1905,7 +1908,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2377,8 +2380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{322C9037-C3F2-41C6-939E-E91FC5A7A254}">
   <dimension ref="A1:O552"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="120" workbookViewId="0">
+      <selection activeCell="C189" sqref="C189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6372,7 +6375,7 @@
         <v>73</v>
       </c>
       <c r="B188" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C188" s="22" t="s">
         <v>164</v>
@@ -6395,7 +6398,7 @@
         <v>73</v>
       </c>
       <c r="B189" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C189" s="22" t="s">
         <v>164</v>
@@ -6416,7 +6419,7 @@
         <v>73</v>
       </c>
       <c r="B190" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C190" s="26" t="s">
         <v>166</v>
@@ -6435,7 +6438,7 @@
         <v>73</v>
       </c>
       <c r="B191" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C191" s="22" t="s">
         <v>8</v>
@@ -6458,7 +6461,7 @@
         <v>73</v>
       </c>
       <c r="B192" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C192" s="22" t="s">
         <v>8</v>
@@ -6481,7 +6484,7 @@
         <v>73</v>
       </c>
       <c r="B193" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C193" s="22" t="s">
         <v>8</v>
@@ -6502,7 +6505,7 @@
         <v>73</v>
       </c>
       <c r="B194" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C194" s="22" t="s">
         <v>8</v>
@@ -6525,7 +6528,7 @@
         <v>73</v>
       </c>
       <c r="B195" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C195" s="22" t="s">
         <v>8</v>
@@ -6548,7 +6551,7 @@
         <v>73</v>
       </c>
       <c r="B196" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C196" s="22" t="s">
         <v>8</v>
@@ -6571,7 +6574,7 @@
         <v>73</v>
       </c>
       <c r="B197" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C197" s="22" t="s">
         <v>8</v>
@@ -6594,7 +6597,7 @@
         <v>73</v>
       </c>
       <c r="B198" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C198" s="22" t="s">
         <v>8</v>
@@ -6615,7 +6618,7 @@
         <v>73</v>
       </c>
       <c r="B199" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C199" s="26" t="s">
         <v>19</v>
@@ -6634,7 +6637,7 @@
         <v>73</v>
       </c>
       <c r="B200" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C200" s="22" t="s">
         <v>38</v>
@@ -6657,7 +6660,7 @@
         <v>73</v>
       </c>
       <c r="B201" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C201" s="22" t="s">
         <v>38</v>
@@ -6678,7 +6681,7 @@
         <v>73</v>
       </c>
       <c r="B202" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C202" s="26" t="s">
         <v>40</v>
@@ -6697,7 +6700,7 @@
         <v>73</v>
       </c>
       <c r="B203" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C203" s="22" t="s">
         <v>20</v>
@@ -6720,7 +6723,7 @@
         <v>73</v>
       </c>
       <c r="B204" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C204" s="22" t="s">
         <v>20</v>
@@ -6743,7 +6746,7 @@
         <v>73</v>
       </c>
       <c r="B205" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C205" s="22" t="s">
         <v>20</v>
@@ -6764,7 +6767,7 @@
         <v>73</v>
       </c>
       <c r="B206" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C206" s="26" t="s">
         <v>24</v>
@@ -6783,7 +6786,7 @@
         <v>73</v>
       </c>
       <c r="B207" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C207" s="22" t="s">
         <v>44</v>
@@ -6806,7 +6809,7 @@
         <v>73</v>
       </c>
       <c r="B208" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C208" s="22" t="s">
         <v>44</v>
@@ -6827,7 +6830,7 @@
         <v>73</v>
       </c>
       <c r="B209" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C209" s="22" t="s">
         <v>44</v>
@@ -6850,7 +6853,7 @@
         <v>73</v>
       </c>
       <c r="B210" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C210" s="22" t="s">
         <v>44</v>
@@ -6871,7 +6874,7 @@
         <v>73</v>
       </c>
       <c r="B211" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C211" s="26" t="s">
         <v>46</v>
@@ -6890,7 +6893,7 @@
         <v>73</v>
       </c>
       <c r="B212" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C212" s="22" t="s">
         <v>47</v>
@@ -6913,7 +6916,7 @@
         <v>73</v>
       </c>
       <c r="B213" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C213" s="22" t="s">
         <v>47</v>
@@ -6936,7 +6939,7 @@
         <v>73</v>
       </c>
       <c r="B214" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C214" s="22" t="s">
         <v>47</v>
@@ -6959,7 +6962,7 @@
         <v>73</v>
       </c>
       <c r="B215" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C215" s="22" t="s">
         <v>47</v>
@@ -6980,7 +6983,7 @@
         <v>73</v>
       </c>
       <c r="B216" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C216" s="22" t="s">
         <v>47</v>
@@ -7003,7 +7006,7 @@
         <v>73</v>
       </c>
       <c r="B217" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C217" s="22" t="s">
         <v>47</v>
@@ -7026,7 +7029,7 @@
         <v>73</v>
       </c>
       <c r="B218" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C218" s="22" t="s">
         <v>47</v>
@@ -7049,7 +7052,7 @@
         <v>73</v>
       </c>
       <c r="B219" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C219" s="22" t="s">
         <v>47</v>
@@ -7072,7 +7075,7 @@
         <v>73</v>
       </c>
       <c r="B220" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C220" s="22" t="s">
         <v>47</v>
@@ -7093,7 +7096,7 @@
         <v>73</v>
       </c>
       <c r="B221" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C221" s="22" t="s">
         <v>47</v>
@@ -7116,7 +7119,7 @@
         <v>73</v>
       </c>
       <c r="B222" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C222" s="22" t="s">
         <v>47</v>
@@ -7139,7 +7142,7 @@
         <v>73</v>
       </c>
       <c r="B223" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C223" s="22" t="s">
         <v>47</v>
@@ -7162,7 +7165,7 @@
         <v>73</v>
       </c>
       <c r="B224" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C224" s="22" t="s">
         <v>47</v>
@@ -7185,7 +7188,7 @@
         <v>73</v>
       </c>
       <c r="B225" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C225" s="22" t="s">
         <v>47</v>
@@ -7206,7 +7209,7 @@
         <v>73</v>
       </c>
       <c r="B226" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C226" s="26" t="s">
         <v>51</v>
@@ -7225,7 +7228,7 @@
         <v>73</v>
       </c>
       <c r="B227" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C227" s="22" t="s">
         <v>52</v>
@@ -7248,7 +7251,7 @@
         <v>73</v>
       </c>
       <c r="B228" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C228" s="22" t="s">
         <v>52</v>
@@ -7271,7 +7274,7 @@
         <v>73</v>
       </c>
       <c r="B229" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C229" s="22" t="s">
         <v>52</v>
@@ -7294,7 +7297,7 @@
         <v>73</v>
       </c>
       <c r="B230" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C230" s="22" t="s">
         <v>52</v>
@@ -7315,7 +7318,7 @@
         <v>73</v>
       </c>
       <c r="B231" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C231" s="26" t="s">
         <v>56</v>
@@ -7334,7 +7337,7 @@
         <v>73</v>
       </c>
       <c r="B232" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C232" s="22" t="s">
         <v>25</v>
@@ -7357,7 +7360,7 @@
         <v>73</v>
       </c>
       <c r="B233" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C233" s="22" t="s">
         <v>25</v>
@@ -7378,7 +7381,7 @@
         <v>73</v>
       </c>
       <c r="B234" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C234" s="22" t="s">
         <v>25</v>
@@ -7401,7 +7404,7 @@
         <v>73</v>
       </c>
       <c r="B235" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C235" s="22" t="s">
         <v>25</v>
@@ -7424,7 +7427,7 @@
         <v>73</v>
       </c>
       <c r="B236" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C236" s="22" t="s">
         <v>25</v>
@@ -7447,7 +7450,7 @@
         <v>73</v>
       </c>
       <c r="B237" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C237" s="22" t="s">
         <v>25</v>
@@ -7468,7 +7471,7 @@
         <v>73</v>
       </c>
       <c r="B238" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C238" s="22" t="s">
         <v>25</v>
@@ -7491,7 +7494,7 @@
         <v>73</v>
       </c>
       <c r="B239" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C239" s="22" t="s">
         <v>25</v>
@@ -7514,7 +7517,7 @@
         <v>73</v>
       </c>
       <c r="B240" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C240" s="22" t="s">
         <v>25</v>
@@ -7537,7 +7540,7 @@
         <v>73</v>
       </c>
       <c r="B241" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C241" s="22" t="s">
         <v>25</v>
@@ -7560,7 +7563,7 @@
         <v>73</v>
       </c>
       <c r="B242" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C242" s="22" t="s">
         <v>25</v>
@@ -7581,7 +7584,7 @@
         <v>73</v>
       </c>
       <c r="B243" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C243" s="26" t="s">
         <v>27</v>
@@ -7600,7 +7603,7 @@
         <v>73</v>
       </c>
       <c r="B244" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C244" s="22" t="s">
         <v>123</v>
@@ -7623,7 +7626,7 @@
         <v>73</v>
       </c>
       <c r="B245" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C245" s="22" t="s">
         <v>123</v>
@@ -7646,7 +7649,7 @@
         <v>73</v>
       </c>
       <c r="B246" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C246" s="22" t="s">
         <v>123</v>
@@ -7667,7 +7670,7 @@
         <v>73</v>
       </c>
       <c r="B247" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C247" s="22" t="s">
         <v>123</v>
@@ -7690,7 +7693,7 @@
         <v>73</v>
       </c>
       <c r="B248" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C248" s="22" t="s">
         <v>123</v>
@@ -7713,7 +7716,7 @@
         <v>73</v>
       </c>
       <c r="B249" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C249" s="22" t="s">
         <v>123</v>
@@ -7736,7 +7739,7 @@
         <v>73</v>
       </c>
       <c r="B250" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C250" s="22" t="s">
         <v>123</v>
@@ -7757,7 +7760,7 @@
         <v>73</v>
       </c>
       <c r="B251" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C251" s="22" t="s">
         <v>123</v>
@@ -7780,7 +7783,7 @@
         <v>73</v>
       </c>
       <c r="B252" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C252" s="22" t="s">
         <v>123</v>
@@ -7803,7 +7806,7 @@
         <v>73</v>
       </c>
       <c r="B253" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C253" s="22" t="s">
         <v>123</v>
@@ -7824,7 +7827,7 @@
         <v>73</v>
       </c>
       <c r="B254" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C254" s="26" t="s">
         <v>127</v>
@@ -7843,7 +7846,7 @@
         <v>73</v>
       </c>
       <c r="B255" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C255" s="22" t="s">
         <v>243</v>
@@ -7866,7 +7869,7 @@
         <v>73</v>
       </c>
       <c r="B256" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C256" s="22" t="s">
         <v>243</v>
@@ -7887,7 +7890,7 @@
         <v>73</v>
       </c>
       <c r="B257" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C257" s="26" t="s">
         <v>245</v>
@@ -7906,7 +7909,7 @@
         <v>73</v>
       </c>
       <c r="B258" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C258" s="22" t="s">
         <v>28</v>
@@ -7929,7 +7932,7 @@
         <v>73</v>
       </c>
       <c r="B259" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C259" s="22" t="s">
         <v>28</v>
@@ -7950,7 +7953,7 @@
         <v>73</v>
       </c>
       <c r="B260" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C260" s="22" t="s">
         <v>28</v>
@@ -7973,7 +7976,7 @@
         <v>73</v>
       </c>
       <c r="B261" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C261" s="22" t="s">
         <v>28</v>
@@ -7994,7 +7997,7 @@
         <v>73</v>
       </c>
       <c r="B262" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C262" s="22" t="s">
         <v>28</v>
@@ -8017,7 +8020,7 @@
         <v>73</v>
       </c>
       <c r="B263" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C263" s="22" t="s">
         <v>28</v>
@@ -8038,7 +8041,7 @@
         <v>73</v>
       </c>
       <c r="B264" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C264" s="26" t="s">
         <v>30</v>
@@ -8057,7 +8060,7 @@
         <v>73</v>
       </c>
       <c r="B265" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C265" s="22" t="s">
         <v>61</v>
@@ -8080,7 +8083,7 @@
         <v>73</v>
       </c>
       <c r="B266" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C266" s="22" t="s">
         <v>61</v>
@@ -8103,7 +8106,7 @@
         <v>73</v>
       </c>
       <c r="B267" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C267" s="22" t="s">
         <v>61</v>
@@ -8126,7 +8129,7 @@
         <v>73</v>
       </c>
       <c r="B268" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C268" s="22" t="s">
         <v>61</v>
@@ -8147,7 +8150,7 @@
         <v>73</v>
       </c>
       <c r="B269" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C269" s="22" t="s">
         <v>61</v>
@@ -8170,7 +8173,7 @@
         <v>73</v>
       </c>
       <c r="B270" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C270" s="22" t="s">
         <v>61</v>
@@ -8193,7 +8196,7 @@
         <v>73</v>
       </c>
       <c r="B271" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C271" s="22" t="s">
         <v>61</v>
@@ -8216,7 +8219,7 @@
         <v>73</v>
       </c>
       <c r="B272" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C272" s="22" t="s">
         <v>61</v>
@@ -8237,7 +8240,7 @@
         <v>73</v>
       </c>
       <c r="B273" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C273" s="22" t="s">
         <v>61</v>
@@ -8260,7 +8263,7 @@
         <v>73</v>
       </c>
       <c r="B274" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C274" s="22" t="s">
         <v>61</v>
@@ -8283,7 +8286,7 @@
         <v>73</v>
       </c>
       <c r="B275" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C275" s="22" t="s">
         <v>61</v>
@@ -8304,7 +8307,7 @@
         <v>73</v>
       </c>
       <c r="B276" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C276" s="26" t="s">
         <v>63</v>
@@ -8323,7 +8326,7 @@
         <v>73</v>
       </c>
       <c r="B277" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C277" s="22" t="s">
         <v>258</v>
@@ -8346,7 +8349,7 @@
         <v>73</v>
       </c>
       <c r="B278" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C278" s="22" t="s">
         <v>258</v>
@@ -8367,7 +8370,7 @@
         <v>73</v>
       </c>
       <c r="B279" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C279" s="26" t="s">
         <v>260</v>
@@ -8386,7 +8389,7 @@
         <v>73</v>
       </c>
       <c r="B280" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C280" s="22" t="s">
         <v>129</v>
@@ -8409,7 +8412,7 @@
         <v>73</v>
       </c>
       <c r="B281" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C281" s="22" t="s">
         <v>129</v>
@@ -8430,7 +8433,7 @@
         <v>73</v>
       </c>
       <c r="B282" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C282" s="22" t="s">
         <v>129</v>
@@ -8453,7 +8456,7 @@
         <v>73</v>
       </c>
       <c r="B283" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C283" s="22" t="s">
         <v>129</v>
@@ -8474,7 +8477,7 @@
         <v>73</v>
       </c>
       <c r="B284" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C284" s="26" t="s">
         <v>131</v>
@@ -8493,7 +8496,7 @@
         <v>73</v>
       </c>
       <c r="B285" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C285" s="22" t="s">
         <v>64</v>
@@ -8516,7 +8519,7 @@
         <v>73</v>
       </c>
       <c r="B286" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C286" s="22" t="s">
         <v>64</v>
@@ -8539,7 +8542,7 @@
         <v>73</v>
       </c>
       <c r="B287" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C287" s="22" t="s">
         <v>64</v>
@@ -8560,7 +8563,7 @@
         <v>73</v>
       </c>
       <c r="B288" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C288" s="22" t="s">
         <v>64</v>
@@ -8583,7 +8586,7 @@
         <v>73</v>
       </c>
       <c r="B289" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C289" s="22" t="s">
         <v>64</v>
@@ -8606,7 +8609,7 @@
         <v>73</v>
       </c>
       <c r="B290" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C290" s="22" t="s">
         <v>64</v>
@@ -8627,7 +8630,7 @@
         <v>73</v>
       </c>
       <c r="B291" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C291" s="22" t="s">
         <v>64</v>
@@ -8650,7 +8653,7 @@
         <v>73</v>
       </c>
       <c r="B292" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C292" s="22" t="s">
         <v>64</v>
@@ -8671,7 +8674,7 @@
         <v>73</v>
       </c>
       <c r="B293" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C293" s="26" t="s">
         <v>66</v>
@@ -8690,7 +8693,7 @@
         <v>73</v>
       </c>
       <c r="B294" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C294" s="22" t="s">
         <v>67</v>
@@ -8713,7 +8716,7 @@
         <v>73</v>
       </c>
       <c r="B295" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C295" s="22" t="s">
         <v>67</v>
@@ -8736,7 +8739,7 @@
         <v>73</v>
       </c>
       <c r="B296" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C296" s="22" t="s">
         <v>67</v>
@@ -8757,7 +8760,7 @@
         <v>73</v>
       </c>
       <c r="B297" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C297" s="22" t="s">
         <v>67</v>
@@ -8780,7 +8783,7 @@
         <v>73</v>
       </c>
       <c r="B298" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C298" s="22" t="s">
         <v>67</v>
@@ -8801,7 +8804,7 @@
         <v>73</v>
       </c>
       <c r="B299" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C299" s="22" t="s">
         <v>67</v>
@@ -8822,7 +8825,7 @@
         <v>73</v>
       </c>
       <c r="B300" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C300" s="22" t="s">
         <v>67</v>
@@ -8845,7 +8848,7 @@
         <v>73</v>
       </c>
       <c r="B301" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C301" s="22" t="s">
         <v>67</v>
@@ -8868,7 +8871,7 @@
         <v>73</v>
       </c>
       <c r="B302" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C302" s="22" t="s">
         <v>67</v>
@@ -8891,7 +8894,7 @@
         <v>73</v>
       </c>
       <c r="B303" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C303" s="22" t="s">
         <v>67</v>
@@ -8914,7 +8917,7 @@
         <v>73</v>
       </c>
       <c r="B304" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C304" s="22" t="s">
         <v>67</v>
@@ -8935,7 +8938,7 @@
         <v>73</v>
       </c>
       <c r="B305" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C305" s="26" t="s">
         <v>69</v>
@@ -8954,7 +8957,7 @@
         <v>73</v>
       </c>
       <c r="B306" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C306" s="22" t="s">
         <v>70</v>
@@ -8977,7 +8980,7 @@
         <v>73</v>
       </c>
       <c r="B307" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C307" s="22" t="s">
         <v>70</v>
@@ -8998,7 +9001,7 @@
         <v>73</v>
       </c>
       <c r="B308" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C308" s="22" t="s">
         <v>70</v>
@@ -9021,7 +9024,7 @@
         <v>73</v>
       </c>
       <c r="B309" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C309" s="22" t="s">
         <v>70</v>
@@ -9042,7 +9045,7 @@
         <v>73</v>
       </c>
       <c r="B310" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C310" s="22" t="s">
         <v>70</v>
@@ -9065,7 +9068,7 @@
         <v>73</v>
       </c>
       <c r="B311" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C311" s="22" t="s">
         <v>70</v>
@@ -9088,7 +9091,7 @@
         <v>73</v>
       </c>
       <c r="B312" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C312" s="22" t="s">
         <v>70</v>
@@ -9109,7 +9112,7 @@
         <v>73</v>
       </c>
       <c r="B313" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C313" s="26" t="s">
         <v>72</v>
@@ -9128,7 +9131,7 @@
         <v>73</v>
       </c>
       <c r="B314" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C314" s="22" t="s">
         <v>288</v>
@@ -9151,7 +9154,7 @@
         <v>73</v>
       </c>
       <c r="B315" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C315" s="22" t="s">
         <v>288</v>
@@ -9174,7 +9177,7 @@
         <v>73</v>
       </c>
       <c r="B316" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C316" s="22" t="s">
         <v>288</v>
@@ -9195,7 +9198,7 @@
         <v>73</v>
       </c>
       <c r="B317" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C317" s="22" t="s">
         <v>288</v>
@@ -9218,7 +9221,7 @@
         <v>73</v>
       </c>
       <c r="B318" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C318" s="22" t="s">
         <v>288</v>
@@ -9239,7 +9242,7 @@
         <v>73</v>
       </c>
       <c r="B319" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C319" s="26" t="s">
         <v>293</v>
@@ -9258,7 +9261,7 @@
         <v>73</v>
       </c>
       <c r="B320" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C320" s="22" t="s">
         <v>295</v>
@@ -9281,7 +9284,7 @@
         <v>73</v>
       </c>
       <c r="B321" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C321" s="22" t="s">
         <v>295</v>
@@ -9302,7 +9305,7 @@
         <v>73</v>
       </c>
       <c r="B322" s="22" t="s">
-        <v>144</v>
+        <v>458</v>
       </c>
       <c r="C322" s="26" t="s">
         <v>297</v>

</xml_diff>